<commit_message>
add combine and change theme
</commit_message>
<xml_diff>
--- a/upload/group1.xlsx
+++ b/upload/group1.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Assignments" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -428,120 +428,68 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
-    <col width="59" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="19" customWidth="1" min="1" max="1"/>
+    <col width="59" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="14" customWidth="1" min="7" max="7"/>
-    <col width="8" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>group_file</t>
+          <t>channel</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>channel</t>
+          <t>directory</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>directory</t>
+          <t>title</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>description</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>publish_date</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>publish_date</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
           <t>publish_time</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>mode</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>group1.csv</t>
+          <t>P-20250927_105039</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P-20250927_105039</t>
+          <t>\\nashp\DATABUHP\Nam SEO\.KhaiThacShort\Number B\232G.mp4</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\nashp\DATABUHP\Nam SEO\.KhaiThacShort\Number B\291G.mp4</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>gagasha</t>
-        </is>
-      </c>
+          <t>fasgsagas</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>titles</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>group1.csv</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>P-20250925_041637</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>\\nashp\DATABUHP\Nam SEO\.KhaiThacShort\Number B\297G.mp4</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>jgjkagna</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>titles</t>
-        </is>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H3"/>
+  <autoFilter ref="A1:F2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change theme color, fix error with ttk
</commit_message>
<xml_diff>
--- a/upload/group1.xlsx
+++ b/upload/group1.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Assignments" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$15</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -430,7 +430,7 @@
   <cols>
     <col width="19" customWidth="1" min="1" max="1"/>
     <col width="59" customWidth="1" min="2" max="2"/>
-    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="75" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
@@ -468,28 +468,22 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>P-20250927_105039</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>\\nashp\DATABUHP\Nam SEO\.KhaiThacShort\Number B\232G.mp4</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>fasgsagas</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
   </sheetData>
-  <autoFilter ref="A1:F2"/>
+  <autoFilter ref="A1:F15"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add move to new folder collumn
</commit_message>
<xml_diff>
--- a/upload/group1.xlsx
+++ b/upload/group1.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Assignments" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -429,8 +429,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="19" customWidth="1" min="1" max="1"/>
-    <col width="59" customWidth="1" min="2" max="2"/>
-    <col width="75" customWidth="1" min="3" max="3"/>
+    <col width="58" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
@@ -469,21 +469,8 @@
       </c>
     </row>
     <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
   </sheetData>
-  <autoFilter ref="A1:F15"/>
+  <autoFilter ref="A1:F2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add tracking move folder
</commit_message>
<xml_diff>
--- a/upload/group1.xlsx
+++ b/upload/group1.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Assignments" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$11</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -429,8 +429,8 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="19" customWidth="1" min="1" max="1"/>
-    <col width="58" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="59" customWidth="1" min="2" max="2"/>
+    <col width="80" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
@@ -468,9 +468,8 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
   </sheetData>
-  <autoFilter ref="A1:F2"/>
+  <autoFilter ref="A1:F11"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>